<commit_message>
Project Plan - Updated
</commit_message>
<xml_diff>
--- a/project-mgmt/docs/CHHS-ADPQ-Project Plan.xlsx
+++ b/project-mgmt/docs/CHHS-ADPQ-Project Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="95">
   <si>
     <t>Sno.</t>
   </si>
@@ -237,9 +237,6 @@
     <t>REGRESSION TEST CASE EXECUTION</t>
   </si>
   <si>
-    <t>BUG FIXIN</t>
-  </si>
-  <si>
     <t>STABILIZATION</t>
   </si>
   <si>
@@ -264,28 +261,12 @@
     <t>DEFINE CHECKIN GUIDELINE</t>
   </si>
   <si>
-    <t>Amit Sharma, Naveen, Ajit</t>
-  </si>
-  <si>
-    <t>Ajit</t>
-  </si>
-  <si>
-    <t>Amit Sharma, Ajit</t>
-  </si>
-  <si>
     <t>AUTO BUILD</t>
   </si>
   <si>
-    <t>Amit Sharma , Ajit</t>
-  </si>
-  <si>
     <t>Rahul B , Vaibhav, Amit Sikka</t>
   </si>
   <si>
-    <t>Amit Sharma, Ajit, Rahul B, 
-Vishal</t>
-  </si>
-  <si>
     <t>Documentation</t>
   </si>
   <si>
@@ -302,12 +283,6 @@
   </si>
   <si>
     <t>COMPLETED</t>
-  </si>
-  <si>
-    <t>IN PROGRESS</t>
-  </si>
-  <si>
-    <t>NOT STARTED</t>
   </si>
   <si>
     <t>Date of
@@ -334,6 +309,24 @@
   </si>
   <si>
     <t>On HOLD</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Amit Sharma, Manish, Rahul B, Vishal</t>
+  </si>
+  <si>
+    <t>Amit Sharma, Naveen, Manish</t>
+  </si>
+  <si>
+    <t>Manish</t>
+  </si>
+  <si>
+    <t>Amit Sharma, Manish</t>
+  </si>
+  <si>
+    <t>Amit Sharma , Manish</t>
   </si>
 </sst>
 </file>
@@ -373,7 +366,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,12 +394,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -486,7 +473,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -783,8 +769,8 @@
   <dimension ref="B3:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +789,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>1</v>
@@ -812,10 +798,10 @@
         <v>2</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>89</v>
+        <v>79</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>6</v>
@@ -841,18 +827,18 @@
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="10"/>
       <c r="F5" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="25">
+        <v>80</v>
+      </c>
+      <c r="G5" s="24">
         <v>42514</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -863,9 +849,9 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="25">
+        <v>80</v>
+      </c>
+      <c r="G6" s="24">
         <v>42514</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -880,9 +866,9 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="25">
+        <v>80</v>
+      </c>
+      <c r="G7" s="24">
         <v>42514</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -897,9 +883,9 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="25">
+        <v>80</v>
+      </c>
+      <c r="G8" s="24">
         <v>42514</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -914,9 +900,9 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="25">
+        <v>80</v>
+      </c>
+      <c r="G9" s="24">
         <v>42514</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -931,9 +917,9 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="25">
+        <v>80</v>
+      </c>
+      <c r="G10" s="24">
         <v>42514</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -948,9 +934,9 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="22"/>
+        <v>88</v>
+      </c>
+      <c r="G11" s="21"/>
       <c r="H11" s="2" t="s">
         <v>18</v>
       </c>
@@ -963,9 +949,9 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="26">
+        <v>80</v>
+      </c>
+      <c r="G12" s="25">
         <v>42515</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -980,9 +966,9 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G13" s="26">
+        <v>80</v>
+      </c>
+      <c r="G13" s="25">
         <v>42516</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -992,14 +978,14 @@
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="25">
+        <v>80</v>
+      </c>
+      <c r="G14" s="24">
         <v>42514</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -1014,9 +1000,9 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="22"/>
+        <v>80</v>
+      </c>
+      <c r="G15" s="21"/>
       <c r="H15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1024,16 +1010,16 @@
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" s="22"/>
+        <v>80</v>
+      </c>
+      <c r="G16" s="21"/>
       <c r="H16" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1044,9 +1030,9 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G17" s="25">
+        <v>80</v>
+      </c>
+      <c r="G17" s="24">
         <v>42515</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -1061,9 +1047,9 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" s="25">
+        <v>80</v>
+      </c>
+      <c r="G18" s="24">
         <v>42515</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -1084,7 +1070,7 @@
         <v>42517</v>
       </c>
       <c r="F19" s="11"/>
-      <c r="G19" s="24"/>
+      <c r="G19" s="23"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1094,10 +1080,12 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="2"/>
+      <c r="F20" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="24">
+        <v>42519</v>
+      </c>
       <c r="H20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1109,10 +1097,12 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="2"/>
+      <c r="F21" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="24">
+        <v>42521</v>
+      </c>
       <c r="H21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1124,10 +1114,12 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="2"/>
+      <c r="F22" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="24">
+        <v>42519</v>
+      </c>
       <c r="H22" s="2" t="s">
         <v>41</v>
       </c>
@@ -1139,10 +1131,12 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="22"/>
+      <c r="F23" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="24">
+        <v>42519</v>
+      </c>
       <c r="H23" s="2" t="s">
         <v>42</v>
       </c>
@@ -1154,10 +1148,12 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="22"/>
+      <c r="F24" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="24">
+        <v>42519</v>
+      </c>
       <c r="H24" s="2" t="s">
         <v>41</v>
       </c>
@@ -1170,9 +1166,9 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G25" s="25">
+        <v>80</v>
+      </c>
+      <c r="G25" s="24">
         <v>42517</v>
       </c>
       <c r="H25" s="2" t="s">
@@ -1187,13 +1183,13 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="25">
+        <v>80</v>
+      </c>
+      <c r="G26" s="24">
         <v>42517</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1204,9 +1200,9 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G27" s="25">
+        <v>80</v>
+      </c>
+      <c r="G27" s="24">
         <v>42517</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -1221,9 +1217,9 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G28" s="25">
+        <v>80</v>
+      </c>
+      <c r="G28" s="24">
         <v>42517</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -1238,13 +1234,13 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G29" s="25">
+        <v>80</v>
+      </c>
+      <c r="G29" s="24">
         <v>42516</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1255,9 +1251,9 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" s="25">
+        <v>80</v>
+      </c>
+      <c r="G30" s="24">
         <v>42518</v>
       </c>
       <c r="H30" s="2" t="s">
@@ -1271,12 +1267,14 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G31" s="2"/>
+      <c r="F31" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" s="24">
+        <v>42523</v>
+      </c>
       <c r="H31" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1286,10 +1284,12 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" s="2"/>
+      <c r="F32" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" s="24">
+        <v>42521</v>
+      </c>
       <c r="H32" s="2" t="s">
         <v>51</v>
       </c>
@@ -1301,10 +1301,12 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G33" s="2"/>
+      <c r="F33" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" s="24">
+        <v>42521</v>
+      </c>
       <c r="H33" s="2" t="s">
         <v>51</v>
       </c>
@@ -1312,14 +1314,16 @@
     <row r="34" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="6" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G34" s="2"/>
+      <c r="F34" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="24">
+        <v>42522</v>
+      </c>
       <c r="H34" s="2" t="s">
         <v>54</v>
       </c>
@@ -1331,10 +1335,12 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G35" s="2"/>
+      <c r="F35" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G35" s="24">
+        <v>42523</v>
+      </c>
       <c r="H35" s="2" t="s">
         <v>58</v>
       </c>
@@ -1347,11 +1353,11 @@
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
       <c r="F36" s="19" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="15" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -1361,12 +1367,12 @@
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
-      <c r="F37" s="20" t="s">
-        <v>87</v>
+      <c r="F37" s="19" t="s">
+        <v>80</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="15" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -1394,9 +1400,9 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G39" s="25">
+        <v>80</v>
+      </c>
+      <c r="G39" s="24">
         <v>42517</v>
       </c>
       <c r="H39" s="2" t="s">
@@ -1427,10 +1433,12 @@
       <c r="E41" s="10">
         <v>42521</v>
       </c>
-      <c r="F41" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G41" s="10"/>
+      <c r="F41" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G41" s="24">
+        <v>42521</v>
+      </c>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -1440,12 +1448,14 @@
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G42" s="2"/>
+      <c r="F42" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="24">
+        <v>42523</v>
+      </c>
       <c r="H42" s="2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -1455,8 +1465,12 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="F43" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G43" s="24">
+        <v>42523</v>
+      </c>
       <c r="H43" s="2" t="s">
         <v>17</v>
       </c>
@@ -1468,10 +1482,14 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="F44" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" s="24">
+        <v>42523</v>
+      </c>
       <c r="H44" s="2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -1481,10 +1499,14 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="F45" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G45" s="24">
+        <v>42523</v>
+      </c>
       <c r="H45" s="2" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
@@ -1494,8 +1516,12 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="F46" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G46" s="24">
+        <v>42523</v>
+      </c>
       <c r="H46" s="2" t="s">
         <v>23</v>
       </c>
@@ -1507,8 +1533,12 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="F47" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G47" s="24">
+        <v>42523</v>
+      </c>
       <c r="H47" s="2" t="s">
         <v>51</v>
       </c>
@@ -1520,21 +1550,29 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="F48" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G48" s="24">
+        <v>42523</v>
+      </c>
       <c r="H48" s="2" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="C49" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
+      <c r="F49" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G49" s="24">
+        <v>42523</v>
+      </c>
       <c r="H49" s="2" t="s">
         <v>16</v>
       </c>
@@ -1559,20 +1597,26 @@
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="F51" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G51" s="24">
+        <v>42521</v>
+      </c>
       <c r="H51" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
+      <c r="F52" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
     </row>
@@ -1598,10 +1642,14 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
+      <c r="F54" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G54" s="24">
+        <v>42525</v>
+      </c>
       <c r="H54" s="2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
@@ -1611,8 +1659,12 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
+      <c r="F55" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G55" s="24">
+        <v>42525</v>
+      </c>
       <c r="H55" s="2" t="s">
         <v>17</v>
       </c>
@@ -1624,10 +1676,14 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="F56" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G56" s="24">
+        <v>42525</v>
+      </c>
       <c r="H56" s="2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
@@ -1637,8 +1693,12 @@
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+      <c r="F57" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G57" s="24">
+        <v>42527</v>
+      </c>
       <c r="H57" s="2" t="s">
         <v>23</v>
       </c>
@@ -1650,10 +1710,14 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
+      <c r="F58" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G58" s="24">
+        <v>42527</v>
+      </c>
       <c r="H58" s="2" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
@@ -1663,8 +1727,12 @@
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
+      <c r="F59" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G59" s="24">
+        <v>42526</v>
+      </c>
       <c r="H59" s="2" t="s">
         <v>51</v>
       </c>
@@ -1676,8 +1744,10 @@
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
+      <c r="F60" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G60" s="24"/>
       <c r="H60" s="2" t="s">
         <v>51</v>
       </c>
@@ -1689,10 +1759,14 @@
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
+      <c r="F61" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G61" s="24">
+        <v>42527</v>
+      </c>
       <c r="H61" s="2" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -1702,8 +1776,12 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
+      <c r="F62" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G62" s="24">
+        <v>42527</v>
+      </c>
       <c r="H62" s="2" t="s">
         <v>16</v>
       </c>
@@ -1715,7 +1793,9 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="F63" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2" t="s">
         <v>16</v>
@@ -1728,16 +1808,20 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
+      <c r="F64" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G64" s="24">
+        <v>42525</v>
+      </c>
       <c r="H64" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D65" s="15"/>
       <c r="E65" s="15"/>
@@ -1750,7 +1834,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -1758,44 +1842,48 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D67" s="11">
         <v>42526</v>
       </c>
       <c r="E67" s="11">
-        <v>42526</v>
-      </c>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>42528</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G67" s="2"/>
+      <c r="H67" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D68" s="11">
-        <v>42526</v>
+        <v>42529</v>
       </c>
       <c r="E68" s="11">
-        <v>42526</v>
-      </c>
-      <c r="F68" s="11"/>
+        <v>42529</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="G68" s="11"/>
-      <c r="H68" s="18" t="s">
-        <v>80</v>
+      <c r="H68" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
@@ -1810,16 +1898,16 @@
       <c r="C70" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D70" s="10">
-        <v>42527</v>
-      </c>
-      <c r="E70" s="10">
-        <v>42527</v>
+      <c r="D70" s="11">
+        <v>42529</v>
+      </c>
+      <c r="E70" s="11">
+        <v>42529</v>
       </c>
       <c r="F70" s="10"/>
       <c r="G70" s="10"/>
       <c r="H70" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
@@ -1827,18 +1915,18 @@
         <v>7</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D71" s="10">
-        <v>42527</v>
-      </c>
-      <c r="E71" s="10">
-        <v>42527</v>
+        <v>70</v>
+      </c>
+      <c r="D71" s="11">
+        <v>42529</v>
+      </c>
+      <c r="E71" s="11">
+        <v>42529</v>
       </c>
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
       <c r="H71" s="2" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
@@ -1846,7 +1934,7 @@
         <v>8</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D72" s="10">
         <v>42526</v>
@@ -1854,8 +1942,12 @@
       <c r="E72" s="10">
         <v>42528</v>
       </c>
-      <c r="F72" s="10"/>
-      <c r="G72" s="10"/>
+      <c r="F72" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G72" s="24">
+        <v>42527</v>
+      </c>
       <c r="H72" s="2" t="s">
         <v>25</v>
       </c>
@@ -1865,18 +1957,18 @@
         <v>9</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D73" s="10">
-        <v>42527</v>
-      </c>
-      <c r="E73" s="10">
-        <v>42527</v>
+        <v>66</v>
+      </c>
+      <c r="D73" s="11">
+        <v>42529</v>
+      </c>
+      <c r="E73" s="11">
+        <v>42529</v>
       </c>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
       <c r="H73" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
@@ -1884,13 +1976,13 @@
         <v>10</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D74" s="17">
-        <v>42528</v>
-      </c>
-      <c r="E74" s="17">
-        <v>42528</v>
+        <v>67</v>
+      </c>
+      <c r="D74" s="11">
+        <v>42530</v>
+      </c>
+      <c r="E74" s="11">
+        <v>42530</v>
       </c>
       <c r="F74" s="17"/>
       <c r="G74" s="17"/>

</xml_diff>

<commit_message>
Project Plan - Updated Tracking 0607
</commit_message>
<xml_diff>
--- a/project-mgmt/docs/CHHS-ADPQ-Project Plan.xlsx
+++ b/project-mgmt/docs/CHHS-ADPQ-Project Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="97">
   <si>
     <t>Sno.</t>
   </si>
@@ -327,6 +327,12 @@
   </si>
   <si>
     <t>Amit Sharma , Manish</t>
+  </si>
+  <si>
+    <t>Revision Backlog Workitems</t>
+  </si>
+  <si>
+    <t>Naveen, Manish</t>
   </si>
 </sst>
 </file>
@@ -766,11 +772,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H74"/>
+  <dimension ref="B3:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
+      <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,40 +1888,40 @@
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D69" s="11">
+        <v>42527</v>
+      </c>
+      <c r="E69" s="11">
+        <v>42528</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G69" s="11"/>
+      <c r="H69" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+      <c r="C70" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="2">
-        <v>6</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D70" s="11">
-        <v>42529</v>
-      </c>
-      <c r="E70" s="11">
-        <v>42529</v>
-      </c>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
-      <c r="H70" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D71" s="11">
         <v>42529</v>
@@ -1926,67 +1932,86 @@
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
       <c r="H71" s="2" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
-        <v>8</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D72" s="10">
-        <v>42526</v>
-      </c>
-      <c r="E72" s="10">
-        <v>42528</v>
-      </c>
-      <c r="F72" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="G72" s="24">
-        <v>42527</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72" s="11">
+        <v>42529</v>
+      </c>
+      <c r="E72" s="11">
+        <v>42529</v>
+      </c>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
       <c r="H72" s="2" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
-        <v>9</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D73" s="11">
-        <v>42529</v>
-      </c>
-      <c r="E73" s="11">
-        <v>42529</v>
-      </c>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D73" s="10">
+        <v>42526</v>
+      </c>
+      <c r="E73" s="10">
+        <v>42528</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G73" s="24">
+        <v>42527</v>
+      </c>
       <c r="H73" s="2" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="2">
+        <v>9</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D74" s="11">
+        <v>42529</v>
+      </c>
+      <c r="E74" s="11">
+        <v>42529</v>
+      </c>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="2">
         <v>10</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="C75" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D74" s="11">
+      <c r="D75" s="11">
         <v>42530</v>
       </c>
-      <c r="E74" s="11">
+      <c r="E75" s="11">
         <v>42530</v>
       </c>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="15" t="s">
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="15" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>